<commit_message>
Tävling Jälla september 2020
</commit_message>
<xml_diff>
--- a/mallar/import/Jalla_september_2020.xlsx
+++ b/mallar/import/Jalla_september_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\episerver\voltige\VoltigeClosedXML\mallar\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCE115D-37E6-46F0-9D11-EAF38C0578F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42C260A-12C5-49CD-B8BD-917E187E07EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="780" windowWidth="29040" windowHeight="17640" xr2:uid="{AB315E71-407A-4084-B7A8-D6D6B844B3A4}"/>
+    <workbookView xWindow="20108" yWindow="2100" windowWidth="2700" windowHeight="1590" xr2:uid="{AB315E71-407A-4084-B7A8-D6D6B844B3A4}"/>
   </bookViews>
   <sheets>
     <sheet name="ekipage" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="236">
   <si>
     <t>Linn Odensten</t>
   </si>
@@ -737,6 +737,15 @@
   </si>
   <si>
     <t>Team Safir</t>
+  </si>
+  <si>
+    <t>47 (2 domare)</t>
+  </si>
+  <si>
+    <t>Tindra Öberg och Lovisa Baeckström</t>
+  </si>
+  <si>
+    <t>Elin Hedman(S)</t>
   </si>
 </sst>
 </file>
@@ -780,7 +789,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -789,6 +798,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1106,8 +1116,8 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:W40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1306,10 +1316,10 @@
         <v>7</v>
       </c>
       <c r="P3">
-        <v>54208</v>
+        <v>109403</v>
       </c>
       <c r="Q3" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="R3">
         <v>41401</v>
@@ -1362,10 +1372,10 @@
         <v>127</v>
       </c>
       <c r="L4">
-        <v>40406</v>
+        <v>99940406</v>
       </c>
       <c r="M4" t="s">
-        <v>18</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.45">
@@ -1417,28 +1427,28 @@
         <v>110</v>
       </c>
       <c r="D6">
-        <v>56148</v>
+        <v>39527</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F6">
-        <v>116676</v>
+        <v>10362</v>
       </c>
       <c r="G6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H6">
-        <v>114</v>
+        <v>875</v>
       </c>
       <c r="I6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L6">
-        <v>56088</v>
+        <v>99523</v>
       </c>
       <c r="M6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.45">
@@ -1452,28 +1462,28 @@
         <v>110</v>
       </c>
       <c r="D7">
-        <v>39527</v>
+        <v>141889</v>
       </c>
       <c r="E7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F7">
-        <v>10362</v>
+        <v>5831</v>
       </c>
       <c r="G7" t="s">
-        <v>84</v>
+        <v>224</v>
       </c>
       <c r="H7">
-        <v>875</v>
+        <v>223</v>
       </c>
       <c r="I7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="L7">
-        <v>99523</v>
+        <v>38739</v>
       </c>
       <c r="M7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.45">
@@ -1496,7 +1506,7 @@
         <v>5831</v>
       </c>
       <c r="G8" t="s">
-        <v>224</v>
+        <v>85</v>
       </c>
       <c r="H8">
         <v>223</v>
@@ -1505,56 +1515,56 @@
         <v>73</v>
       </c>
       <c r="L8">
-        <v>38739</v>
+        <v>40310</v>
       </c>
       <c r="M8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>490705</v>
+        <v>490707</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D9">
-        <v>141889</v>
+        <v>56148</v>
       </c>
       <c r="E9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F9">
-        <v>5831</v>
+        <v>116676</v>
       </c>
       <c r="G9" t="s">
-        <v>85</v>
+        <v>228</v>
       </c>
       <c r="H9">
-        <v>223</v>
+        <v>114</v>
       </c>
       <c r="I9" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="L9">
-        <v>40310</v>
+        <v>124198</v>
       </c>
       <c r="M9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>490707</v>
+        <v>490705</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D10">
         <v>56148</v>
@@ -1566,7 +1576,7 @@
         <v>116676</v>
       </c>
       <c r="G10" t="s">
-        <v>228</v>
+        <v>83</v>
       </c>
       <c r="H10">
         <v>114</v>
@@ -1575,10 +1585,10 @@
         <v>76</v>
       </c>
       <c r="L10">
-        <v>124198</v>
+        <v>56088</v>
       </c>
       <c r="M10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.45">
@@ -1661,7 +1671,7 @@
       <c r="C13" t="s">
         <v>112</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4">
         <v>56148</v>
       </c>
       <c r="E13" t="s">
@@ -1706,7 +1716,7 @@
         <v>2135</v>
       </c>
       <c r="G14" t="s">
-        <v>223</v>
+        <v>86</v>
       </c>
       <c r="H14">
         <v>875</v>
@@ -1715,13 +1725,13 @@
         <v>77</v>
       </c>
       <c r="J14" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="L14">
-        <v>119967</v>
+        <v>99453</v>
       </c>
       <c r="M14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.45">
@@ -1735,31 +1745,31 @@
         <v>112</v>
       </c>
       <c r="D15">
-        <v>36847</v>
+        <v>49704</v>
       </c>
       <c r="E15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F15">
-        <v>81736</v>
+        <v>2135</v>
       </c>
       <c r="G15" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="H15">
-        <v>223</v>
+        <v>875</v>
       </c>
       <c r="I15" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="J15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L15">
-        <v>74165</v>
+        <v>119967</v>
       </c>
       <c r="M15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.45">
@@ -1773,31 +1783,31 @@
         <v>112</v>
       </c>
       <c r="D16">
-        <v>49704</v>
+        <v>36847</v>
       </c>
       <c r="E16" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F16">
-        <v>2135</v>
+        <v>81736</v>
       </c>
       <c r="G16" t="s">
-        <v>86</v>
+        <v>229</v>
       </c>
       <c r="H16">
-        <v>875</v>
+        <v>223</v>
       </c>
       <c r="I16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L16">
-        <v>99453</v>
+        <v>74165</v>
       </c>
       <c r="M16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.45">
@@ -2053,14 +2063,11 @@
       <c r="I23" t="s">
         <v>73</v>
       </c>
-      <c r="J23" t="s">
-        <v>137</v>
-      </c>
       <c r="L23">
-        <v>145200</v>
+        <v>101580</v>
       </c>
       <c r="M23" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.45">
@@ -2080,10 +2087,10 @@
         <v>101</v>
       </c>
       <c r="F24">
-        <v>81736</v>
+        <v>93110</v>
       </c>
       <c r="G24" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H24">
         <v>223</v>
@@ -2092,13 +2099,13 @@
         <v>73</v>
       </c>
       <c r="J24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L24">
-        <v>134608</v>
+        <v>145200</v>
       </c>
       <c r="M24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.45">
@@ -2112,31 +2119,31 @@
         <v>113</v>
       </c>
       <c r="D25">
-        <v>39527</v>
+        <v>36847</v>
       </c>
       <c r="E25" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F25">
-        <v>10362</v>
+        <v>81736</v>
       </c>
       <c r="G25" t="s">
-        <v>226</v>
+        <v>87</v>
       </c>
       <c r="H25">
-        <v>875</v>
+        <v>223</v>
       </c>
       <c r="I25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L25">
-        <v>107672</v>
+        <v>134608</v>
       </c>
       <c r="M25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.45">
@@ -2150,28 +2157,31 @@
         <v>113</v>
       </c>
       <c r="D26">
-        <v>36847</v>
+        <v>39527</v>
       </c>
       <c r="E26" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F26">
-        <v>93110</v>
+        <v>10362</v>
       </c>
       <c r="G26" t="s">
-        <v>90</v>
+        <v>226</v>
       </c>
       <c r="H26">
-        <v>223</v>
+        <v>875</v>
       </c>
       <c r="I26" t="s">
-        <v>73</v>
+        <v>77</v>
+      </c>
+      <c r="J26" t="s">
+        <v>139</v>
       </c>
       <c r="L26">
-        <v>101580</v>
+        <v>107672</v>
       </c>
       <c r="M26" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.45">
@@ -2223,64 +2233,58 @@
         <v>116</v>
       </c>
       <c r="D28">
-        <v>36847</v>
+        <v>95073</v>
       </c>
       <c r="E28" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F28">
-        <v>81736</v>
+        <v>55525</v>
       </c>
       <c r="G28" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="H28">
-        <v>223</v>
+        <v>1198</v>
       </c>
       <c r="I28" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="K28" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="L28">
-        <v>134608</v>
+        <v>133914</v>
       </c>
       <c r="M28" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="N28">
-        <v>150025</v>
+        <v>141722</v>
       </c>
       <c r="O28" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="P28">
-        <v>145287</v>
+        <v>129688</v>
       </c>
       <c r="Q28" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="R28">
-        <v>149851</v>
+        <v>129079</v>
       </c>
       <c r="S28" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="T28">
-        <v>160950</v>
+        <v>163768</v>
       </c>
       <c r="U28" t="s">
-        <v>38</v>
-      </c>
-      <c r="V28">
-        <v>150091</v>
-      </c>
-      <c r="W28" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.45">
@@ -2294,64 +2298,64 @@
         <v>116</v>
       </c>
       <c r="D29">
-        <v>68838</v>
+        <v>36847</v>
       </c>
       <c r="E29" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F29">
-        <v>137228</v>
+        <v>81736</v>
       </c>
       <c r="G29" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H29">
-        <v>875</v>
+        <v>223</v>
       </c>
       <c r="I29" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L29">
-        <v>36794</v>
+        <v>134608</v>
       </c>
       <c r="M29" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="N29">
-        <v>50023</v>
+        <v>150025</v>
       </c>
       <c r="O29" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="P29">
-        <v>64245</v>
+        <v>145287</v>
       </c>
       <c r="Q29" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="R29">
-        <v>82678</v>
+        <v>149851</v>
       </c>
       <c r="S29" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="T29">
-        <v>64250</v>
+        <v>160950</v>
       </c>
       <c r="U29" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="V29">
-        <v>108189</v>
+        <v>150091</v>
       </c>
       <c r="W29" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.45">
@@ -2365,58 +2369,64 @@
         <v>116</v>
       </c>
       <c r="D30">
-        <v>95073</v>
+        <v>68838</v>
       </c>
       <c r="E30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F30">
-        <v>55525</v>
+        <v>137228</v>
       </c>
       <c r="G30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H30">
-        <v>1198</v>
+        <v>875</v>
       </c>
       <c r="I30" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="J30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L30">
-        <v>133914</v>
+        <v>36794</v>
       </c>
       <c r="M30" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="N30">
-        <v>141722</v>
+        <v>50023</v>
       </c>
       <c r="O30" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="P30">
-        <v>129688</v>
+        <v>64245</v>
       </c>
       <c r="Q30" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="R30">
-        <v>129079</v>
+        <v>82678</v>
       </c>
       <c r="S30" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="T30">
-        <v>163768</v>
+        <v>64250</v>
       </c>
       <c r="U30" t="s">
-        <v>50</v>
+        <v>44</v>
+      </c>
+      <c r="V30">
+        <v>108189</v>
+      </c>
+      <c r="W30" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.45">
@@ -2430,58 +2440,58 @@
         <v>117</v>
       </c>
       <c r="D31">
-        <v>56148</v>
+        <v>40068</v>
       </c>
       <c r="E31" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F31">
-        <v>133922</v>
+        <v>72506</v>
       </c>
       <c r="G31" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="H31">
-        <v>114</v>
+        <v>223</v>
       </c>
       <c r="I31" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J31" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K31" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="L31">
-        <v>152168</v>
+        <v>158594</v>
       </c>
       <c r="M31" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="N31">
-        <v>141313</v>
+        <v>163832</v>
       </c>
       <c r="O31" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="P31">
-        <v>129556</v>
+        <v>148007</v>
       </c>
       <c r="Q31" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="R31">
-        <v>129524</v>
+        <v>163903</v>
       </c>
       <c r="S31" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="T31">
-        <v>129417</v>
+        <v>150090</v>
       </c>
       <c r="U31" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.45">
@@ -2495,58 +2505,58 @@
         <v>117</v>
       </c>
       <c r="D32">
-        <v>40068</v>
+        <v>56148</v>
       </c>
       <c r="E32" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F32">
-        <v>72506</v>
+        <v>133922</v>
       </c>
       <c r="G32" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="H32">
-        <v>223</v>
+        <v>114</v>
       </c>
       <c r="I32" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="J32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K32" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L32">
-        <v>158594</v>
+        <v>152168</v>
       </c>
       <c r="M32" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="N32">
-        <v>163832</v>
+        <v>141313</v>
       </c>
       <c r="O32" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P32">
-        <v>148007</v>
+        <v>129556</v>
       </c>
       <c r="Q32" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="R32">
-        <v>163903</v>
+        <v>129524</v>
       </c>
       <c r="S32" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="T32">
-        <v>150090</v>
+        <v>129417</v>
       </c>
       <c r="U32" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.45">
@@ -2560,52 +2570,46 @@
         <v>119</v>
       </c>
       <c r="D33">
-        <v>163755</v>
+        <v>40310</v>
       </c>
       <c r="E33" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="F33">
-        <v>98871</v>
+        <v>93110</v>
       </c>
       <c r="G33" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H33">
-        <v>114</v>
+        <v>223</v>
       </c>
       <c r="I33" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J33" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="K33" t="s">
-        <v>232</v>
+        <v>148</v>
       </c>
       <c r="L33">
-        <v>130297</v>
+        <v>155140</v>
       </c>
       <c r="M33" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="N33">
-        <v>155892</v>
+        <v>164021</v>
       </c>
       <c r="O33" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="P33">
-        <v>163872</v>
+        <v>164010</v>
       </c>
       <c r="Q33" t="s">
-        <v>63</v>
-      </c>
-      <c r="R33">
-        <v>160597</v>
-      </c>
-      <c r="S33" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.45">
@@ -2619,52 +2623,52 @@
         <v>119</v>
       </c>
       <c r="D34">
-        <v>54511</v>
+        <v>163755</v>
       </c>
       <c r="E34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F34">
-        <v>72506</v>
+        <v>98871</v>
       </c>
       <c r="G34" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="H34">
-        <v>223</v>
+        <v>114</v>
       </c>
       <c r="I34" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="J34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K34" t="s">
-        <v>147</v>
+        <v>232</v>
       </c>
       <c r="L34">
-        <v>163943</v>
+        <v>130297</v>
       </c>
       <c r="M34" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="N34">
-        <v>163765</v>
+        <v>155892</v>
       </c>
       <c r="O34" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="P34">
-        <v>155344</v>
+        <v>163872</v>
       </c>
       <c r="Q34" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="R34">
-        <v>164011</v>
+        <v>160597</v>
       </c>
       <c r="S34" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.45">
@@ -2678,16 +2682,16 @@
         <v>119</v>
       </c>
       <c r="D35">
-        <v>40310</v>
+        <v>54511</v>
       </c>
       <c r="E35" t="s">
-        <v>22</v>
+        <v>106</v>
       </c>
       <c r="F35">
-        <v>93110</v>
+        <v>72506</v>
       </c>
       <c r="G35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H35">
         <v>223</v>
@@ -2696,28 +2700,34 @@
         <v>73</v>
       </c>
       <c r="J35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L35">
-        <v>155140</v>
+        <v>163943</v>
       </c>
       <c r="M35" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="N35">
-        <v>164021</v>
+        <v>163765</v>
       </c>
       <c r="O35" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="P35">
-        <v>164010</v>
+        <v>155344</v>
       </c>
       <c r="Q35" t="s">
-        <v>71</v>
+        <v>67</v>
+      </c>
+      <c r="R35">
+        <v>164011</v>
+      </c>
+      <c r="S35" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.45">
@@ -2787,13 +2797,13 @@
         <v>76</v>
       </c>
       <c r="J37" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="L37">
-        <v>160597</v>
+        <v>130297</v>
       </c>
       <c r="M37" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.45">
@@ -2860,13 +2870,13 @@
         <v>76</v>
       </c>
       <c r="J39" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L39">
-        <v>130297</v>
+        <v>160597</v>
       </c>
       <c r="M39" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.45">
@@ -2880,10 +2890,10 @@
         <v>123</v>
       </c>
       <c r="D40">
-        <v>36847</v>
+        <v>40310</v>
       </c>
       <c r="E40" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="F40">
         <v>93110</v>
@@ -2899,6 +2909,9 @@
       </c>
       <c r="J40" t="s">
         <v>135</v>
+      </c>
+      <c r="K40" t="s">
+        <v>234</v>
       </c>
       <c r="L40">
         <v>101407</v>
@@ -2924,7 +2937,7 @@
   <dimension ref="A1:Q53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3143,10 +3156,13 @@
         <v>116</v>
       </c>
       <c r="D10">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="E10">
         <v>1054</v>
+      </c>
+      <c r="G10">
+        <v>1053</v>
       </c>
       <c r="O10" s="1">
         <v>18</v>
@@ -3169,10 +3185,13 @@
         <v>117</v>
       </c>
       <c r="D11">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
         <v>152</v>
+      </c>
+      <c r="G11" t="s">
+        <v>233</v>
       </c>
       <c r="O11" s="1">
         <v>19</v>
@@ -3215,10 +3234,13 @@
         <v>119</v>
       </c>
       <c r="D13">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E13" t="s">
         <v>153</v>
+      </c>
+      <c r="G13">
+        <v>44</v>
       </c>
       <c r="O13" s="1">
         <v>21</v>
@@ -3261,10 +3283,13 @@
         <v>121</v>
       </c>
       <c r="D15">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E15">
         <v>48</v>
+      </c>
+      <c r="G15">
+        <v>43</v>
       </c>
       <c r="O15" s="1">
         <v>23</v>
@@ -3287,10 +3312,13 @@
         <v>122</v>
       </c>
       <c r="D16">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E16">
         <v>49</v>
+      </c>
+      <c r="G16">
+        <v>45</v>
       </c>
       <c r="O16" s="1">
         <v>24</v>
@@ -3313,10 +3341,13 @@
         <v>123</v>
       </c>
       <c r="D17">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="E17">
         <v>1056</v>
+      </c>
+      <c r="G17">
+        <v>1055</v>
       </c>
       <c r="O17" s="1">
         <v>25</v>
@@ -4073,10 +4104,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A28B307A-344C-405A-B58D-A87B55F418A9}">
   <sheetPr codeName="Blad6"/>
-  <dimension ref="A1:B73"/>
+  <dimension ref="A1:B74"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4665,6 +4696,14 @@
         <v>72</v>
       </c>
     </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A74">
+        <v>99940406</v>
+      </c>
+      <c r="B74" t="s">
+        <v>235</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>